<commit_message>
Adding pdf data and updated pubs.csv file
</commit_message>
<xml_diff>
--- a/scraped_data/analysis_pubs.xlsx
+++ b/scraped_data/analysis_pubs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniela\Documents\Repositories\scholarlyScrape\scraped_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E3C32F-D6F9-419D-BE13-E0C7F453EDBD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01DB77A-E27A-4C7D-81EA-57329BF07D72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-120" windowWidth="28080" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15930" yWindow="8610" windowWidth="20880" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pubs" sheetId="3" r:id="rId1"/>
@@ -6936,7 +6936,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7116,6 +7116,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -7277,9 +7283,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -9784,18 +9791,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D85D1FD9-025B-4B4D-9F2B-AF31DAC1BE5F}">
   <dimension ref="A1:I476"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="A394" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A367" sqref="A367"/>
+      <selection pane="topRight" activeCell="A400" sqref="A400"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.5703125" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="42.7109375" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
@@ -11976,728 +11985,728 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="76" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
         <v>1100</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="2" t="s">
         <v>1101</v>
       </c>
-      <c r="C76">
+      <c r="C76" s="2">
         <v>2008</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" s="2" t="s">
         <v>1102</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="2" t="s">
         <v>1103</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F76" s="2" t="s">
         <v>1104</v>
       </c>
-      <c r="G76">
+      <c r="G76" s="2">
         <v>149</v>
       </c>
-      <c r="H76">
+      <c r="H76" s="2">
         <v>613</v>
       </c>
-      <c r="I76" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="I76" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
         <v>1105</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="2" t="s">
         <v>1106</v>
       </c>
-      <c r="C77">
+      <c r="C77" s="2">
         <v>2001</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="2" t="s">
         <v>1107</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F77" s="2" t="s">
         <v>1108</v>
       </c>
-      <c r="G77">
+      <c r="G77" s="2">
         <v>151</v>
       </c>
-      <c r="H77">
+      <c r="H77" s="2">
         <v>329</v>
       </c>
-      <c r="I77" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="I77" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
         <v>1109</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="2" t="s">
         <v>1110</v>
       </c>
-      <c r="C78">
+      <c r="C78" s="2">
         <v>2008</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" s="2" t="s">
         <v>1111</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E78" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F78" s="2" t="s">
         <v>1112</v>
       </c>
-      <c r="G78">
+      <c r="G78" s="2">
         <v>153</v>
       </c>
-      <c r="H78">
+      <c r="H78" s="2">
         <v>684</v>
       </c>
-      <c r="I78" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="I78" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
         <v>1113</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C79">
+      <c r="C79" s="2">
         <v>2017</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D79" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F79" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="G79">
+      <c r="G79" s="2">
         <v>155</v>
       </c>
-      <c r="H79">
+      <c r="H79" s="2">
         <v>43</v>
       </c>
-      <c r="I79" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="I79" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
         <v>1114</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C80">
+      <c r="C80" s="2">
         <v>2017</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D80" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E80" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F80" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="G80">
+      <c r="G80" s="2">
         <v>157</v>
       </c>
-      <c r="H80">
+      <c r="H80" s="2">
         <v>138</v>
       </c>
-      <c r="I80" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="I80" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
         <v>1115</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C81">
+      <c r="C81" s="2">
         <v>2012</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D81" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E81" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F81" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="G81">
+      <c r="G81" s="2">
         <v>159</v>
       </c>
-      <c r="H81">
+      <c r="H81" s="2">
         <v>100</v>
       </c>
-      <c r="I81" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="I81" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
         <v>1116</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C82">
+      <c r="C82" s="2">
         <v>2016</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D82" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E82" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F82" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="G82">
+      <c r="G82" s="2">
         <v>161</v>
       </c>
-      <c r="H82">
+      <c r="H82" s="2">
         <v>472</v>
       </c>
-      <c r="I82" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="I82" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
         <v>1117</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C83">
+      <c r="C83" s="2">
         <v>2014</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D83" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E83" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F83" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="G83">
+      <c r="G83" s="2">
         <v>163</v>
       </c>
-      <c r="H83">
+      <c r="H83" s="2">
         <v>14</v>
       </c>
-      <c r="I83" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="I83" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
         <v>1118</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C84">
+      <c r="C84" s="2">
         <v>2008</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D84" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E84" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F84" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="G84">
+      <c r="G84" s="2">
         <v>165</v>
       </c>
-      <c r="H84">
+      <c r="H84" s="2">
         <v>564</v>
       </c>
-      <c r="I84" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="I84" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
         <v>1119</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C85">
+      <c r="C85" s="2">
         <v>2018</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D85" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E85" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="F85" t="s">
+      <c r="F85" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="G85">
+      <c r="G85" s="2">
         <v>167</v>
       </c>
-      <c r="H85">
+      <c r="H85" s="2">
         <v>137</v>
       </c>
-      <c r="I85" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="I85" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
         <v>1120</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="2" t="s">
         <v>1121</v>
       </c>
-      <c r="C86">
+      <c r="C86" s="2">
         <v>2013</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D86" s="2" t="s">
         <v>1122</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E86" s="2" t="s">
         <v>1123</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F86" s="2" t="s">
         <v>1124</v>
       </c>
-      <c r="G86">
+      <c r="G86" s="2">
         <v>169</v>
       </c>
-      <c r="H86">
+      <c r="H86" s="2">
         <v>8</v>
       </c>
-      <c r="I86" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+      <c r="I86" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
         <v>1125</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="2" t="s">
         <v>1126</v>
       </c>
-      <c r="C87">
+      <c r="C87" s="2">
         <v>2012</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" s="2" t="s">
         <v>1127</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E87" s="2" t="s">
         <v>1128</v>
       </c>
-      <c r="F87" t="s">
+      <c r="F87" s="2" t="s">
         <v>1129</v>
       </c>
-      <c r="G87">
+      <c r="G87" s="2">
         <v>171</v>
       </c>
-      <c r="H87">
+      <c r="H87" s="2">
         <v>172</v>
       </c>
-      <c r="I87" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="I87" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
         <v>1130</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="2" t="s">
         <v>1131</v>
       </c>
-      <c r="C88">
+      <c r="C88" s="2">
         <v>2016</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D88" s="2" t="s">
         <v>1132</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E88" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F88" t="s">
+      <c r="F88" s="2" t="s">
         <v>1133</v>
       </c>
-      <c r="G88">
+      <c r="G88" s="2">
         <v>173</v>
       </c>
-      <c r="H88">
+      <c r="H88" s="2">
         <v>120</v>
       </c>
-      <c r="I88" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="I88" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
         <v>1134</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="2" t="s">
         <v>1135</v>
       </c>
-      <c r="C89">
+      <c r="C89" s="2">
         <v>2010</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D89" s="2" t="s">
         <v>1136</v>
       </c>
-      <c r="E89" t="s">
+      <c r="E89" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F89" t="s">
+      <c r="F89" s="2" t="s">
         <v>1137</v>
       </c>
-      <c r="G89">
+      <c r="G89" s="2">
         <v>175</v>
       </c>
-      <c r="H89">
+      <c r="H89" s="2">
         <v>165</v>
       </c>
-      <c r="I89" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="I89" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
         <v>1138</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="2" t="s">
         <v>662</v>
       </c>
-      <c r="C90">
+      <c r="C90" s="2">
         <v>2019</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D90" s="2" t="s">
         <v>663</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E90" s="2" t="s">
         <v>664</v>
       </c>
-      <c r="F90" t="s">
+      <c r="F90" s="2" t="s">
         <v>665</v>
       </c>
-      <c r="G90">
+      <c r="G90" s="2">
         <v>177</v>
       </c>
-      <c r="H90">
+      <c r="H90" s="2">
         <v>6</v>
       </c>
-      <c r="I90" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="I90" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
         <v>1139</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="2" t="s">
         <v>1140</v>
       </c>
-      <c r="C91">
+      <c r="C91" s="2">
         <v>2017</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D91" s="2" t="s">
         <v>1141</v>
       </c>
-      <c r="E91" t="s">
+      <c r="E91" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F91" t="s">
+      <c r="F91" s="2" t="s">
         <v>1142</v>
       </c>
-      <c r="G91">
+      <c r="G91" s="2">
         <v>179</v>
       </c>
-      <c r="H91">
+      <c r="H91" s="2">
         <v>29</v>
       </c>
-      <c r="I91" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+      <c r="I91" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
         <v>1143</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="2" t="s">
         <v>666</v>
       </c>
-      <c r="C92">
+      <c r="C92" s="2">
         <v>2009</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="2" t="s">
         <v>667</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E92" s="2" t="s">
         <v>668</v>
       </c>
-      <c r="F92" t="s">
+      <c r="F92" s="2" t="s">
         <v>669</v>
       </c>
-      <c r="G92">
+      <c r="G92" s="2">
         <v>181</v>
       </c>
-      <c r="H92">
+      <c r="H92" s="2">
         <v>60</v>
       </c>
-      <c r="I92" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="I92" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
         <v>1144</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="2" t="s">
         <v>670</v>
       </c>
-      <c r="C93">
+      <c r="C93" s="2">
         <v>2019</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93" s="2" t="s">
         <v>671</v>
       </c>
-      <c r="E93" t="s">
+      <c r="E93" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="F93" t="s">
+      <c r="F93" s="2" t="s">
         <v>673</v>
       </c>
-      <c r="G93">
+      <c r="G93" s="2">
         <v>183</v>
       </c>
-      <c r="H93">
+      <c r="H93" s="2">
         <v>35</v>
       </c>
-      <c r="I93" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="I93" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
         <v>1145</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="2" t="s">
         <v>674</v>
       </c>
-      <c r="C94">
+      <c r="C94" s="2">
         <v>2011</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="2" t="s">
         <v>675</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E94" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F94" t="s">
+      <c r="F94" s="2" t="s">
         <v>676</v>
       </c>
-      <c r="G94">
+      <c r="G94" s="2">
         <v>185</v>
       </c>
-      <c r="H94">
+      <c r="H94" s="2">
         <v>48</v>
       </c>
-      <c r="I94" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="I94" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
         <v>1146</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="2" t="s">
         <v>677</v>
       </c>
-      <c r="C95">
+      <c r="C95" s="2">
         <v>2019</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D95" s="2" t="s">
         <v>678</v>
       </c>
-      <c r="E95" t="s">
+      <c r="E95" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="F95" t="s">
+      <c r="F95" s="2" t="s">
         <v>679</v>
       </c>
-      <c r="G95">
+      <c r="G95" s="2">
         <v>187</v>
       </c>
-      <c r="H95">
+      <c r="H95" s="2">
         <v>31</v>
       </c>
-      <c r="I95" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="I95" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
         <v>1147</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="2" t="s">
         <v>680</v>
       </c>
-      <c r="C96">
+      <c r="C96" s="2">
         <v>2015</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="2" t="s">
         <v>681</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E96" s="2" t="s">
         <v>682</v>
       </c>
-      <c r="F96" t="s">
+      <c r="F96" s="2" t="s">
         <v>683</v>
       </c>
-      <c r="G96">
+      <c r="G96" s="2">
         <v>189</v>
       </c>
-      <c r="H96">
+      <c r="H96" s="2">
         <v>18</v>
       </c>
-      <c r="I96" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="I96" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
         <v>1148</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="2" t="s">
         <v>684</v>
       </c>
-      <c r="C97">
+      <c r="C97" s="2">
         <v>2001</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="2" t="s">
         <v>685</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E97" s="2" t="s">
         <v>686</v>
       </c>
-      <c r="F97" t="s">
+      <c r="F97" s="2" t="s">
         <v>687</v>
       </c>
-      <c r="G97">
+      <c r="G97" s="2">
         <v>191</v>
       </c>
-      <c r="H97">
+      <c r="H97" s="2">
         <v>99</v>
       </c>
-      <c r="I97" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="I97" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
         <v>1149</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="2" t="s">
         <v>688</v>
       </c>
-      <c r="C98">
+      <c r="C98" s="2">
         <v>2014</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="2" t="s">
         <v>689</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E98" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="F98" t="s">
+      <c r="F98" s="2" t="s">
         <v>690</v>
       </c>
-      <c r="G98">
+      <c r="G98" s="2">
         <v>193</v>
       </c>
-      <c r="H98">
+      <c r="H98" s="2">
         <v>68</v>
       </c>
-      <c r="I98" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="I98" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
         <v>1150</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="2" t="s">
         <v>691</v>
       </c>
-      <c r="C99">
+      <c r="C99" s="2">
         <v>2013</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" s="2" t="s">
         <v>692</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E99" s="2" t="s">
         <v>693</v>
       </c>
-      <c r="F99" t="s">
+      <c r="F99" s="2" t="s">
         <v>694</v>
       </c>
-      <c r="G99">
+      <c r="G99" s="2">
         <v>195</v>
       </c>
-      <c r="H99">
+      <c r="H99" s="2">
         <v>6</v>
       </c>
-      <c r="I99" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="I99" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
         <v>1151</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C100">
+      <c r="C100" s="2">
         <v>2013</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E100" t="s">
+      <c r="E100" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F100" t="s">
+      <c r="F100" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="G100">
+      <c r="G100" s="2">
         <v>197</v>
       </c>
-      <c r="H100">
+      <c r="H100" s="2">
         <v>315</v>
       </c>
-      <c r="I100" t="s">
+      <c r="I100" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -14876,728 +14885,728 @@
         <v>13</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
+    <row r="176" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="s">
         <v>1379</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B176" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C176">
+      <c r="C176" s="2">
         <v>2018</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D176" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="E176" t="s">
+      <c r="E176" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="F176" t="s">
+      <c r="F176" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="G176">
+      <c r="G176" s="2">
         <v>349</v>
       </c>
-      <c r="H176">
+      <c r="H176" s="2">
         <v>54</v>
       </c>
-      <c r="I176" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
+      <c r="I176" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="2" t="s">
         <v>1380</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B177" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="C177">
+      <c r="C177" s="2">
         <v>2015</v>
       </c>
-      <c r="D177" t="s">
+      <c r="D177" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="E177" t="s">
+      <c r="E177" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="F177" t="s">
+      <c r="F177" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="G177">
+      <c r="G177" s="2">
         <v>351</v>
       </c>
-      <c r="H177">
+      <c r="H177" s="2">
         <v>22</v>
       </c>
-      <c r="I177" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
+      <c r="I177" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="2" t="s">
         <v>1381</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B178" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="C178">
+      <c r="C178" s="2">
         <v>2015</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D178" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="E178" t="s">
+      <c r="E178" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="F178" t="s">
+      <c r="F178" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="G178">
+      <c r="G178" s="2">
         <v>353</v>
       </c>
-      <c r="H178">
+      <c r="H178" s="2">
         <v>9</v>
       </c>
-      <c r="I178" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
+      <c r="I178" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="2" t="s">
         <v>1382</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B179" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="C179">
+      <c r="C179" s="2">
         <v>2018</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D179" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="E179" t="s">
+      <c r="E179" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="F179" t="s">
+      <c r="F179" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="G179">
+      <c r="G179" s="2">
         <v>355</v>
       </c>
-      <c r="H179">
+      <c r="H179" s="2">
         <v>65</v>
       </c>
-      <c r="I179" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
+      <c r="I179" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A180" s="2" t="s">
         <v>1383</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B180" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="C180">
+      <c r="C180" s="2">
         <v>2008</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D180" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E180" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F180" t="s">
+      <c r="F180" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="G180">
+      <c r="G180" s="2">
         <v>357</v>
       </c>
-      <c r="H180">
+      <c r="H180" s="2">
         <v>20</v>
       </c>
-      <c r="I180" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
+      <c r="I180" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="2" t="s">
         <v>1384</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B181" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="C181">
+      <c r="C181" s="2">
         <v>2019</v>
       </c>
-      <c r="D181" t="s">
+      <c r="D181" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="E181" t="s">
+      <c r="E181" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="F181" t="s">
+      <c r="F181" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="G181">
+      <c r="G181" s="2">
         <v>359</v>
       </c>
-      <c r="H181">
+      <c r="H181" s="2">
         <v>15</v>
       </c>
-      <c r="I181" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
+      <c r="I181" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="2" t="s">
         <v>1385</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B182" s="2" t="s">
         <v>1386</v>
       </c>
-      <c r="C182">
+      <c r="C182" s="2">
         <v>2008</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D182" s="2" t="s">
         <v>1387</v>
       </c>
-      <c r="E182" t="s">
+      <c r="E182" s="2" t="s">
         <v>1388</v>
       </c>
-      <c r="F182" t="s">
+      <c r="F182" s="2" t="s">
         <v>1389</v>
       </c>
-      <c r="G182">
+      <c r="G182" s="2">
         <v>361</v>
       </c>
-      <c r="H182">
-        <v>13</v>
-      </c>
-      <c r="I182" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
+      <c r="H182" s="2">
+        <v>13</v>
+      </c>
+      <c r="I182" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="2" t="s">
         <v>1390</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B183" s="2" t="s">
         <v>737</v>
       </c>
-      <c r="C183">
+      <c r="C183" s="2">
         <v>2008</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D183" s="2" t="s">
         <v>738</v>
       </c>
-      <c r="E183" t="s">
+      <c r="E183" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F183" t="s">
+      <c r="F183" s="2" t="s">
         <v>739</v>
       </c>
-      <c r="G183">
+      <c r="G183" s="2">
         <v>363</v>
       </c>
-      <c r="H183">
+      <c r="H183" s="2">
         <v>83</v>
       </c>
-      <c r="I183" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
+      <c r="I183" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="2" t="s">
         <v>1391</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B184" s="2" t="s">
         <v>740</v>
       </c>
-      <c r="C184">
+      <c r="C184" s="2">
         <v>2009</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D184" s="2" t="s">
         <v>741</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E184" s="2" t="s">
         <v>742</v>
       </c>
-      <c r="F184" t="s">
+      <c r="F184" s="2" t="s">
         <v>743</v>
       </c>
-      <c r="G184">
+      <c r="G184" s="2">
         <v>365</v>
       </c>
-      <c r="H184">
+      <c r="H184" s="2">
         <v>86</v>
       </c>
-      <c r="I184" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
+      <c r="I184" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="2" t="s">
         <v>1392</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B185" s="2" t="s">
         <v>744</v>
       </c>
-      <c r="C185">
+      <c r="C185" s="2">
         <v>2017</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D185" s="2" t="s">
         <v>745</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E185" s="2" t="s">
         <v>746</v>
       </c>
-      <c r="F185" t="s">
+      <c r="F185" s="2" t="s">
         <v>747</v>
       </c>
-      <c r="G185">
+      <c r="G185" s="2">
         <v>367</v>
       </c>
-      <c r="H185">
+      <c r="H185" s="2">
         <v>18</v>
       </c>
-      <c r="I185" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
+      <c r="I185" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="2" t="s">
         <v>1393</v>
       </c>
-      <c r="B186" t="s">
+      <c r="B186" s="2" t="s">
         <v>748</v>
       </c>
-      <c r="C186">
+      <c r="C186" s="2">
         <v>2020</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D186" s="2" t="s">
         <v>749</v>
       </c>
-      <c r="E186" t="s">
+      <c r="E186" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F186" t="s">
+      <c r="F186" s="2" t="s">
         <v>750</v>
       </c>
-      <c r="G186">
+      <c r="G186" s="2">
         <v>369</v>
       </c>
-      <c r="H186">
+      <c r="H186" s="2">
         <v>12</v>
       </c>
-      <c r="I186" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
+      <c r="I186" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="2" t="s">
         <v>1394</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B187" s="2" t="s">
         <v>751</v>
       </c>
-      <c r="C187">
+      <c r="C187" s="2">
         <v>2012</v>
       </c>
-      <c r="D187" t="s">
+      <c r="D187" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="E187" t="s">
+      <c r="E187" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="F187" t="s">
+      <c r="F187" s="2" t="s">
         <v>754</v>
       </c>
-      <c r="G187">
+      <c r="G187" s="2">
         <v>371</v>
       </c>
-      <c r="H187">
+      <c r="H187" s="2">
         <v>42</v>
       </c>
-      <c r="I187" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
+      <c r="I187" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="2" t="s">
         <v>1395</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B188" s="2" t="s">
         <v>1396</v>
       </c>
-      <c r="C188">
+      <c r="C188" s="2">
         <v>2015</v>
       </c>
-      <c r="D188" t="s">
+      <c r="D188" s="2" t="s">
         <v>1397</v>
       </c>
-      <c r="E188" t="s">
+      <c r="E188" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F188" t="s">
+      <c r="F188" s="2" t="s">
         <v>1398</v>
       </c>
-      <c r="G188">
+      <c r="G188" s="2">
         <v>373</v>
       </c>
-      <c r="H188">
+      <c r="H188" s="2">
         <v>3</v>
       </c>
-      <c r="I188" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
+      <c r="I188" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="2" t="s">
         <v>1399</v>
       </c>
-      <c r="B189" t="s">
+      <c r="B189" s="2" t="s">
         <v>1400</v>
       </c>
-      <c r="C189">
+      <c r="C189" s="2">
         <v>2011</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D189" s="2" t="s">
         <v>1401</v>
       </c>
-      <c r="E189" t="s">
+      <c r="E189" s="2" t="s">
         <v>1402</v>
       </c>
-      <c r="F189" t="s">
+      <c r="F189" s="2" t="s">
         <v>1403</v>
       </c>
-      <c r="G189">
+      <c r="G189" s="2">
         <v>375</v>
       </c>
-      <c r="H189">
+      <c r="H189" s="2">
         <v>72</v>
       </c>
-      <c r="I189" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
+      <c r="I189" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="2" t="s">
         <v>1404</v>
       </c>
-      <c r="B190" t="s">
+      <c r="B190" s="2" t="s">
         <v>1405</v>
       </c>
-      <c r="C190">
+      <c r="C190" s="2">
         <v>2005</v>
       </c>
-      <c r="D190" t="s">
+      <c r="D190" s="2" t="s">
         <v>1406</v>
       </c>
-      <c r="E190" t="s">
+      <c r="E190" s="2" t="s">
         <v>1407</v>
       </c>
-      <c r="F190" t="s">
+      <c r="F190" s="2" t="s">
         <v>1408</v>
       </c>
-      <c r="G190">
+      <c r="G190" s="2">
         <v>377</v>
       </c>
-      <c r="H190">
+      <c r="H190" s="2">
         <v>134</v>
       </c>
-      <c r="I190" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
+      <c r="I190" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
         <v>1409</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B191" s="2" t="s">
         <v>1410</v>
       </c>
-      <c r="C191">
+      <c r="C191" s="2">
         <v>2014</v>
       </c>
-      <c r="D191" t="s">
+      <c r="D191" s="2" t="s">
         <v>1411</v>
       </c>
-      <c r="E191" t="s">
+      <c r="E191" s="2" t="s">
         <v>1412</v>
       </c>
-      <c r="F191" t="s">
+      <c r="F191" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="G191">
+      <c r="G191" s="2">
         <v>379</v>
       </c>
-      <c r="H191">
+      <c r="H191" s="2">
         <v>121</v>
       </c>
-      <c r="I191" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
+      <c r="I191" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="2" t="s">
         <v>1414</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B192" s="2" t="s">
         <v>1415</v>
       </c>
-      <c r="C192">
+      <c r="C192" s="2">
         <v>2019</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D192" s="2" t="s">
         <v>1416</v>
       </c>
-      <c r="E192" t="s">
+      <c r="E192" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="F192" t="s">
+      <c r="F192" s="2" t="s">
         <v>1417</v>
       </c>
-      <c r="G192">
+      <c r="G192" s="2">
         <v>381</v>
       </c>
-      <c r="H192">
+      <c r="H192" s="2">
         <v>14</v>
       </c>
-      <c r="I192" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
+      <c r="I192" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="2" t="s">
         <v>1418</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B193" s="2" t="s">
         <v>1419</v>
       </c>
-      <c r="C193">
+      <c r="C193" s="2">
         <v>2005</v>
       </c>
-      <c r="D193" t="s">
+      <c r="D193" s="2" t="s">
         <v>1420</v>
       </c>
-      <c r="E193" t="s">
+      <c r="E193" s="2" t="s">
         <v>1421</v>
       </c>
-      <c r="F193" t="s">
+      <c r="F193" s="2" t="s">
         <v>1422</v>
       </c>
-      <c r="G193">
+      <c r="G193" s="2">
         <v>383</v>
       </c>
-      <c r="H193">
+      <c r="H193" s="2">
         <v>449</v>
       </c>
-      <c r="I193" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
+      <c r="I193" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="2" t="s">
         <v>1423</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B194" s="2" t="s">
         <v>1424</v>
       </c>
-      <c r="C194">
+      <c r="C194" s="2">
         <v>2016</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D194" s="2" t="s">
         <v>1425</v>
       </c>
-      <c r="E194" t="s">
+      <c r="E194" s="2" t="s">
         <v>1426</v>
       </c>
-      <c r="F194" t="s">
+      <c r="F194" s="2" t="s">
         <v>1427</v>
       </c>
-      <c r="G194">
+      <c r="G194" s="2">
         <v>385</v>
       </c>
-      <c r="H194">
+      <c r="H194" s="2">
         <v>7</v>
       </c>
-      <c r="I194" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
+      <c r="I194" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="2" t="s">
         <v>1428</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B195" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="C195">
+      <c r="C195" s="2">
         <v>2011</v>
       </c>
-      <c r="D195" t="s">
+      <c r="D195" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="E195" t="s">
+      <c r="E195" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="F195" t="s">
+      <c r="F195" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="G195">
+      <c r="G195" s="2">
         <v>387</v>
       </c>
-      <c r="H195">
+      <c r="H195" s="2">
         <v>42</v>
       </c>
-      <c r="I195" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
+      <c r="I195" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="2" t="s">
         <v>1429</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B196" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C196">
+      <c r="C196" s="2">
         <v>2016</v>
       </c>
-      <c r="D196" t="s">
+      <c r="D196" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="E196" t="s">
+      <c r="E196" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="F196" t="s">
+      <c r="F196" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="G196">
+      <c r="G196" s="2">
         <v>389</v>
       </c>
-      <c r="H196">
+      <c r="H196" s="2">
         <v>185</v>
       </c>
-      <c r="I196" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
+      <c r="I196" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A197" s="2" t="s">
         <v>1430</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B197" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="C197">
+      <c r="C197" s="2">
         <v>2019</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D197" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="E197" t="s">
+      <c r="E197" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="F197" t="s">
+      <c r="F197" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="G197">
+      <c r="G197" s="2">
         <v>391</v>
       </c>
-      <c r="H197">
+      <c r="H197" s="2">
         <v>7</v>
       </c>
-      <c r="I197" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
+      <c r="I197" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A198" s="2" t="s">
         <v>1431</v>
       </c>
-      <c r="B198" t="s">
+      <c r="B198" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="C198">
+      <c r="C198" s="2">
         <v>2012</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D198" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="E198" t="s">
+      <c r="E198" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="F198" t="s">
+      <c r="F198" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="G198">
+      <c r="G198" s="2">
         <v>393</v>
       </c>
-      <c r="H198">
+      <c r="H198" s="2">
         <v>574</v>
       </c>
-      <c r="I198" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
+      <c r="I198" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="2" t="s">
         <v>1432</v>
       </c>
-      <c r="B199" t="s">
+      <c r="B199" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="C199">
+      <c r="C199" s="2">
         <v>2010</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D199" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="E199" t="s">
+      <c r="E199" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="F199" t="s">
+      <c r="F199" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="G199">
+      <c r="G199" s="2">
         <v>395</v>
       </c>
-      <c r="H199">
+      <c r="H199" s="2">
         <v>149</v>
       </c>
-      <c r="I199" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
+      <c r="I199" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="2" t="s">
         <v>1433</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B200" s="2" t="s">
         <v>1434</v>
       </c>
-      <c r="C200">
+      <c r="C200" s="2">
         <v>2017</v>
       </c>
-      <c r="D200" t="s">
+      <c r="D200" s="2" t="s">
         <v>1435</v>
       </c>
-      <c r="E200" t="s">
+      <c r="E200" s="2" t="s">
         <v>1436</v>
       </c>
-      <c r="F200" t="s">
+      <c r="F200" s="2" t="s">
         <v>1437</v>
       </c>
-      <c r="G200">
+      <c r="G200" s="2">
         <v>397</v>
       </c>
-      <c r="H200">
+      <c r="H200" s="2">
         <v>10</v>
       </c>
-      <c r="I200" t="s">
+      <c r="I200" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -17776,728 +17785,728 @@
         <v>13</v>
       </c>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A276" t="s">
+    <row r="276" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A276" s="2" t="s">
         <v>1706</v>
       </c>
-      <c r="B276" t="s">
+      <c r="B276" s="2" t="s">
         <v>767</v>
       </c>
-      <c r="C276">
+      <c r="C276" s="2">
         <v>2017</v>
       </c>
-      <c r="D276" t="s">
+      <c r="D276" s="2" t="s">
         <v>768</v>
       </c>
-      <c r="E276" t="s">
+      <c r="E276" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="F276" t="s">
+      <c r="F276" s="2" t="s">
         <v>769</v>
       </c>
-      <c r="G276">
+      <c r="G276" s="2">
         <v>549</v>
       </c>
-      <c r="H276">
+      <c r="H276" s="2">
         <v>313</v>
       </c>
-      <c r="I276" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A277" t="s">
+      <c r="I276" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="277" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A277" s="2" t="s">
         <v>1707</v>
       </c>
-      <c r="B277" t="s">
+      <c r="B277" s="2" t="s">
         <v>770</v>
       </c>
-      <c r="C277">
+      <c r="C277" s="2">
         <v>2006</v>
       </c>
-      <c r="D277" t="s">
+      <c r="D277" s="2" t="s">
         <v>771</v>
       </c>
-      <c r="E277" t="s">
+      <c r="E277" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F277" t="s">
+      <c r="F277" s="2" t="s">
         <v>772</v>
       </c>
-      <c r="G277">
+      <c r="G277" s="2">
         <v>551</v>
       </c>
-      <c r="H277">
+      <c r="H277" s="2">
         <v>55</v>
       </c>
-      <c r="I277" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A278" t="s">
+      <c r="I277" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="278" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A278" s="2" t="s">
         <v>1708</v>
       </c>
-      <c r="B278" t="s">
+      <c r="B278" s="2" t="s">
         <v>773</v>
       </c>
-      <c r="C278">
+      <c r="C278" s="2">
         <v>2015</v>
       </c>
-      <c r="D278" t="s">
+      <c r="D278" s="2" t="s">
         <v>774</v>
       </c>
-      <c r="E278" t="s">
+      <c r="E278" s="2" t="s">
         <v>775</v>
       </c>
-      <c r="F278" t="s">
+      <c r="F278" s="2" t="s">
         <v>776</v>
       </c>
-      <c r="G278">
+      <c r="G278" s="2">
         <v>553</v>
       </c>
-      <c r="H278">
+      <c r="H278" s="2">
         <v>30</v>
       </c>
-      <c r="I278" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A279" t="s">
+      <c r="I278" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="279" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A279" s="2" t="s">
         <v>1709</v>
       </c>
-      <c r="B279" t="s">
+      <c r="B279" s="2" t="s">
         <v>777</v>
       </c>
-      <c r="C279">
+      <c r="C279" s="2">
         <v>2007</v>
       </c>
-      <c r="D279" t="s">
+      <c r="D279" s="2" t="s">
         <v>778</v>
       </c>
-      <c r="E279" t="s">
+      <c r="E279" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="F279" t="s">
+      <c r="F279" s="2" t="s">
         <v>779</v>
       </c>
-      <c r="G279">
+      <c r="G279" s="2">
         <v>555</v>
       </c>
-      <c r="H279">
+      <c r="H279" s="2">
         <v>47</v>
       </c>
-      <c r="I279" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A280" t="s">
+      <c r="I279" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="280" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A280" s="2" t="s">
         <v>1710</v>
       </c>
-      <c r="B280" t="s">
+      <c r="B280" s="2" t="s">
         <v>780</v>
       </c>
-      <c r="C280">
+      <c r="C280" s="2">
         <v>2017</v>
       </c>
-      <c r="D280" t="s">
+      <c r="D280" s="2" t="s">
         <v>781</v>
       </c>
-      <c r="E280" t="s">
+      <c r="E280" s="2" t="s">
         <v>782</v>
       </c>
-      <c r="F280" t="s">
+      <c r="F280" s="2" t="s">
         <v>783</v>
       </c>
-      <c r="G280">
+      <c r="G280" s="2">
         <v>557</v>
       </c>
-      <c r="H280">
+      <c r="H280" s="2">
         <v>31</v>
       </c>
-      <c r="I280" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A281" t="s">
+      <c r="I280" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="281" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A281" s="2" t="s">
         <v>1711</v>
       </c>
-      <c r="B281" t="s">
+      <c r="B281" s="2" t="s">
         <v>784</v>
       </c>
-      <c r="C281">
+      <c r="C281" s="2">
         <v>2012</v>
       </c>
-      <c r="D281" t="s">
+      <c r="D281" s="2" t="s">
         <v>785</v>
       </c>
-      <c r="E281" t="s">
+      <c r="E281" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F281" t="s">
+      <c r="F281" s="2" t="s">
         <v>786</v>
       </c>
-      <c r="G281">
+      <c r="G281" s="2">
         <v>559</v>
       </c>
-      <c r="H281">
+      <c r="H281" s="2">
         <v>52</v>
       </c>
-      <c r="I281" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A282" t="s">
+      <c r="I281" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="282" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A282" s="2" t="s">
         <v>1712</v>
       </c>
-      <c r="B282" t="s">
+      <c r="B282" s="2" t="s">
         <v>787</v>
       </c>
-      <c r="C282">
+      <c r="C282" s="2">
         <v>2006</v>
       </c>
-      <c r="D282" t="s">
+      <c r="D282" s="2" t="s">
         <v>788</v>
       </c>
-      <c r="E282" t="s">
+      <c r="E282" s="2" t="s">
         <v>789</v>
       </c>
-      <c r="F282" t="s">
+      <c r="F282" s="2" t="s">
         <v>790</v>
       </c>
-      <c r="G282">
+      <c r="G282" s="2">
         <v>561</v>
       </c>
-      <c r="H282">
+      <c r="H282" s="2">
         <v>33</v>
       </c>
-      <c r="I282" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A283" t="s">
+      <c r="I282" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="283" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A283" s="2" t="s">
         <v>1713</v>
       </c>
-      <c r="B283" t="s">
+      <c r="B283" s="2" t="s">
         <v>791</v>
       </c>
-      <c r="C283">
+      <c r="C283" s="2">
         <v>2019</v>
       </c>
-      <c r="D283" t="s">
+      <c r="D283" s="2" t="s">
         <v>792</v>
       </c>
-      <c r="E283" t="s">
+      <c r="E283" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="F283" t="s">
+      <c r="F283" s="2" t="s">
         <v>793</v>
       </c>
-      <c r="G283">
+      <c r="G283" s="2">
         <v>563</v>
       </c>
-      <c r="H283">
+      <c r="H283" s="2">
         <v>8</v>
       </c>
-      <c r="I283" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A284" t="s">
+      <c r="I283" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="284" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A284" s="2" t="s">
         <v>1714</v>
       </c>
-      <c r="B284" t="s">
+      <c r="B284" s="2" t="s">
         <v>794</v>
       </c>
-      <c r="C284">
+      <c r="C284" s="2">
         <v>2006</v>
       </c>
-      <c r="D284" t="s">
+      <c r="D284" s="2" t="s">
         <v>795</v>
       </c>
-      <c r="E284" t="s">
+      <c r="E284" s="2" t="s">
         <v>796</v>
       </c>
-      <c r="F284" t="s">
+      <c r="F284" s="2" t="s">
         <v>797</v>
       </c>
-      <c r="G284">
+      <c r="G284" s="2">
         <v>565</v>
       </c>
-      <c r="H284">
+      <c r="H284" s="2">
         <v>108</v>
       </c>
-      <c r="I284" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A285" t="s">
+      <c r="I284" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="285" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A285" s="2" t="s">
         <v>1715</v>
       </c>
-      <c r="B285" t="s">
+      <c r="B285" s="2" t="s">
         <v>798</v>
       </c>
-      <c r="C285">
+      <c r="C285" s="2">
         <v>2017</v>
       </c>
-      <c r="D285" t="s">
+      <c r="D285" s="2" t="s">
         <v>799</v>
       </c>
-      <c r="E285" t="s">
+      <c r="E285" s="2" t="s">
         <v>800</v>
       </c>
-      <c r="F285" t="s">
+      <c r="F285" s="2" t="s">
         <v>801</v>
       </c>
-      <c r="G285">
+      <c r="G285" s="2">
         <v>567</v>
       </c>
-      <c r="H285">
+      <c r="H285" s="2">
         <v>32</v>
       </c>
-      <c r="I285" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A286" t="s">
+      <c r="I285" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="286" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A286" s="2" t="s">
         <v>1716</v>
       </c>
-      <c r="B286" t="s">
+      <c r="B286" s="2" t="s">
         <v>1717</v>
       </c>
-      <c r="C286">
+      <c r="C286" s="2">
         <v>2021</v>
       </c>
-      <c r="D286" t="s">
+      <c r="D286" s="2" t="s">
         <v>1718</v>
       </c>
-      <c r="E286" t="s">
+      <c r="E286" s="2" t="s">
         <v>1719</v>
       </c>
-      <c r="F286" t="s">
+      <c r="F286" s="2" t="s">
         <v>1720</v>
       </c>
-      <c r="G286">
+      <c r="G286" s="2">
         <v>569</v>
       </c>
-      <c r="H286">
+      <c r="H286" s="2">
         <v>1</v>
       </c>
-      <c r="I286" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A287" t="s">
+      <c r="I286" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="287" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A287" s="2" t="s">
         <v>1721</v>
       </c>
-      <c r="B287" t="s">
+      <c r="B287" s="2" t="s">
         <v>1722</v>
       </c>
-      <c r="C287">
+      <c r="C287" s="2">
         <v>2016</v>
       </c>
-      <c r="D287" t="s">
+      <c r="D287" s="2" t="s">
         <v>1723</v>
       </c>
-      <c r="E287" t="s">
+      <c r="E287" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F287" t="s">
+      <c r="F287" s="2" t="s">
         <v>1724</v>
       </c>
-      <c r="G287">
+      <c r="G287" s="2">
         <v>571</v>
       </c>
-      <c r="H287">
+      <c r="H287" s="2">
         <v>99</v>
       </c>
-      <c r="I287" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A288" t="s">
+      <c r="I287" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="288" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A288" s="2" t="s">
         <v>1725</v>
       </c>
-      <c r="B288" t="s">
+      <c r="B288" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="C288">
+      <c r="C288" s="2">
         <v>2015</v>
       </c>
-      <c r="D288" t="s">
+      <c r="D288" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="E288" t="s">
+      <c r="E288" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F288" t="s">
+      <c r="F288" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="G288">
+      <c r="G288" s="2">
         <v>573</v>
       </c>
-      <c r="H288">
+      <c r="H288" s="2">
         <v>14</v>
       </c>
-      <c r="I288" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A289" t="s">
+      <c r="I288" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="289" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A289" s="2" t="s">
         <v>1726</v>
       </c>
-      <c r="B289" t="s">
+      <c r="B289" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="C289">
+      <c r="C289" s="2">
         <v>2014</v>
       </c>
-      <c r="D289" t="s">
+      <c r="D289" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="E289" t="s">
+      <c r="E289" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F289" t="s">
+      <c r="F289" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="G289">
+      <c r="G289" s="2">
         <v>575</v>
       </c>
-      <c r="H289">
+      <c r="H289" s="2">
         <v>40</v>
       </c>
-      <c r="I289" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A290" t="s">
+      <c r="I289" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="290" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A290" s="2" t="s">
         <v>1727</v>
       </c>
-      <c r="B290" t="s">
+      <c r="B290" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="C290">
+      <c r="C290" s="2">
         <v>2000</v>
       </c>
-      <c r="D290" t="s">
+      <c r="D290" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="E290" t="s">
+      <c r="E290" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="F290" t="s">
+      <c r="F290" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="G290">
+      <c r="G290" s="2">
         <v>577</v>
       </c>
-      <c r="H290">
+      <c r="H290" s="2">
         <v>15</v>
       </c>
-      <c r="I290" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A291" t="s">
+      <c r="I290" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="291" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A291" s="2" t="s">
         <v>1728</v>
       </c>
-      <c r="B291" t="s">
+      <c r="B291" s="2" t="s">
         <v>1729</v>
       </c>
-      <c r="C291">
+      <c r="C291" s="2">
         <v>2019</v>
       </c>
-      <c r="D291" t="s">
+      <c r="D291" s="2" t="s">
         <v>1730</v>
       </c>
-      <c r="E291" t="s">
+      <c r="E291" s="2" t="s">
         <v>1731</v>
       </c>
-      <c r="F291" t="s">
+      <c r="F291" s="2" t="s">
         <v>1732</v>
       </c>
-      <c r="G291">
+      <c r="G291" s="2">
         <v>579</v>
       </c>
-      <c r="H291">
+      <c r="H291" s="2">
         <v>11</v>
       </c>
-      <c r="I291" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A292" t="s">
+      <c r="I291" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="292" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A292" s="2" t="s">
         <v>1733</v>
       </c>
-      <c r="B292" t="s">
+      <c r="B292" s="2" t="s">
         <v>802</v>
       </c>
-      <c r="C292">
+      <c r="C292" s="2">
         <v>2011</v>
       </c>
-      <c r="D292" t="s">
+      <c r="D292" s="2" t="s">
         <v>803</v>
       </c>
-      <c r="E292" t="s">
+      <c r="E292" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F292" t="s">
+      <c r="F292" s="2" t="s">
         <v>804</v>
       </c>
-      <c r="G292">
+      <c r="G292" s="2">
         <v>581</v>
       </c>
-      <c r="H292">
+      <c r="H292" s="2">
         <v>10</v>
       </c>
-      <c r="I292" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A293" t="s">
+      <c r="I292" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="293" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A293" s="2" t="s">
         <v>1734</v>
       </c>
-      <c r="B293" t="s">
+      <c r="B293" s="2" t="s">
         <v>1735</v>
       </c>
-      <c r="C293">
+      <c r="C293" s="2">
         <v>2021</v>
       </c>
-      <c r="D293" t="s">
+      <c r="D293" s="2" t="s">
         <v>1736</v>
       </c>
-      <c r="E293" t="s">
+      <c r="E293" s="2" t="s">
         <v>1737</v>
       </c>
-      <c r="F293" t="s">
+      <c r="F293" s="2" t="s">
         <v>1738</v>
       </c>
-      <c r="G293">
+      <c r="G293" s="2">
         <v>583</v>
       </c>
-      <c r="H293">
+      <c r="H293" s="2">
         <v>1</v>
       </c>
-      <c r="I293" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A294" t="s">
+      <c r="I293" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="294" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A294" s="2" t="s">
         <v>1739</v>
       </c>
-      <c r="B294" t="s">
+      <c r="B294" s="2" t="s">
         <v>1740</v>
       </c>
-      <c r="C294">
+      <c r="C294" s="2">
         <v>2018</v>
       </c>
-      <c r="D294" t="s">
+      <c r="D294" s="2" t="s">
         <v>1741</v>
       </c>
-      <c r="E294" t="s">
+      <c r="E294" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="F294" t="s">
+      <c r="F294" s="2" t="s">
         <v>1742</v>
       </c>
-      <c r="G294">
+      <c r="G294" s="2">
         <v>585</v>
       </c>
-      <c r="H294">
+      <c r="H294" s="2">
         <v>27</v>
       </c>
-      <c r="I294" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A295" t="s">
+      <c r="I294" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="295" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A295" s="2" t="s">
         <v>1743</v>
       </c>
-      <c r="B295" t="s">
+      <c r="B295" s="2" t="s">
         <v>1744</v>
       </c>
-      <c r="C295">
+      <c r="C295" s="2">
         <v>2013</v>
       </c>
-      <c r="D295" t="s">
+      <c r="D295" s="2" t="s">
         <v>1745</v>
       </c>
-      <c r="E295" t="s">
+      <c r="E295" s="2" t="s">
         <v>1746</v>
       </c>
-      <c r="F295" t="s">
+      <c r="F295" s="2" t="s">
         <v>1747</v>
       </c>
-      <c r="G295">
+      <c r="G295" s="2">
         <v>587</v>
       </c>
-      <c r="H295">
+      <c r="H295" s="2">
         <v>257</v>
       </c>
-      <c r="I295" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A296" t="s">
+      <c r="I295" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="296" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A296" s="2" t="s">
         <v>1748</v>
       </c>
-      <c r="B296" t="s">
+      <c r="B296" s="2" t="s">
         <v>1749</v>
       </c>
-      <c r="C296">
+      <c r="C296" s="2">
         <v>2002</v>
       </c>
-      <c r="D296" t="s">
+      <c r="D296" s="2" t="s">
         <v>1750</v>
       </c>
-      <c r="E296" t="s">
+      <c r="E296" s="2" t="s">
         <v>1751</v>
       </c>
-      <c r="F296" t="s">
+      <c r="F296" s="2" t="s">
         <v>1752</v>
       </c>
-      <c r="G296">
+      <c r="G296" s="2">
         <v>589</v>
       </c>
-      <c r="H296">
+      <c r="H296" s="2">
         <v>729</v>
       </c>
-      <c r="I296" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A297" t="s">
+      <c r="I296" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="297" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A297" s="2" t="s">
         <v>1753</v>
       </c>
-      <c r="B297" t="s">
+      <c r="B297" s="2" t="s">
         <v>1754</v>
       </c>
-      <c r="C297">
+      <c r="C297" s="2">
         <v>2017</v>
       </c>
-      <c r="D297" t="s">
+      <c r="D297" s="2" t="s">
         <v>1755</v>
       </c>
-      <c r="E297" t="s">
+      <c r="E297" s="2" t="s">
         <v>1756</v>
       </c>
-      <c r="F297" t="s">
+      <c r="F297" s="2" t="s">
         <v>1757</v>
       </c>
-      <c r="G297">
+      <c r="G297" s="2">
         <v>591</v>
       </c>
-      <c r="H297">
+      <c r="H297" s="2">
         <v>33</v>
       </c>
-      <c r="I297" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A298" t="s">
+      <c r="I297" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="298" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A298" s="2" t="s">
         <v>1758</v>
       </c>
-      <c r="B298" t="s">
+      <c r="B298" s="2" t="s">
         <v>1759</v>
       </c>
-      <c r="C298">
+      <c r="C298" s="2">
         <v>2008</v>
       </c>
-      <c r="D298" t="s">
+      <c r="D298" s="2" t="s">
         <v>1760</v>
       </c>
-      <c r="E298" t="s">
+      <c r="E298" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F298" t="s">
+      <c r="F298" s="2" t="s">
         <v>1761</v>
       </c>
-      <c r="G298">
+      <c r="G298" s="2">
         <v>593</v>
       </c>
-      <c r="H298">
+      <c r="H298" s="2">
         <v>37</v>
       </c>
-      <c r="I298" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A299" t="s">
+      <c r="I298" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="299" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A299" s="2" t="s">
         <v>1762</v>
       </c>
-      <c r="B299" t="s">
+      <c r="B299" s="2" t="s">
         <v>1763</v>
       </c>
-      <c r="C299">
+      <c r="C299" s="2">
         <v>2009</v>
       </c>
-      <c r="D299" t="s">
+      <c r="D299" s="2" t="s">
         <v>1764</v>
       </c>
-      <c r="E299" t="s">
+      <c r="E299" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F299" t="s">
+      <c r="F299" s="2" t="s">
         <v>1765</v>
       </c>
-      <c r="G299">
+      <c r="G299" s="2">
         <v>595</v>
       </c>
-      <c r="H299">
+      <c r="H299" s="2">
         <v>378</v>
       </c>
-      <c r="I299" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A300" t="s">
+      <c r="I299" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="300" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A300" s="2" t="s">
         <v>1766</v>
       </c>
-      <c r="B300" t="s">
+      <c r="B300" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="C300">
+      <c r="C300" s="2">
         <v>2015</v>
       </c>
-      <c r="D300" t="s">
+      <c r="D300" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="E300" t="s">
+      <c r="E300" s="2" t="s">
         <v>1767</v>
       </c>
-      <c r="F300" t="s">
+      <c r="F300" s="2" t="s">
         <v>1768</v>
       </c>
-      <c r="G300">
+      <c r="G300" s="2">
         <v>597</v>
       </c>
-      <c r="H300">
+      <c r="H300" s="2">
         <v>107</v>
       </c>
-      <c r="I300" t="s">
+      <c r="I300" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -20676,728 +20685,728 @@
         <v>13</v>
       </c>
     </row>
-    <row r="376" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A376" t="s">
+    <row r="376" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A376" s="2" t="s">
         <v>1954</v>
       </c>
-      <c r="B376" t="s">
+      <c r="B376" s="2" t="s">
         <v>870</v>
       </c>
-      <c r="C376">
+      <c r="C376" s="2">
         <v>2012</v>
       </c>
-      <c r="D376" t="s">
+      <c r="D376" s="2" t="s">
         <v>871</v>
       </c>
-      <c r="E376" t="s">
+      <c r="E376" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F376" t="s">
+      <c r="F376" s="2" t="s">
         <v>872</v>
       </c>
-      <c r="G376">
+      <c r="G376" s="2">
         <v>749</v>
       </c>
-      <c r="H376">
+      <c r="H376" s="2">
         <v>3</v>
       </c>
-      <c r="I376" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="377" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A377" t="s">
+      <c r="I376" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="377" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A377" s="2" t="s">
         <v>1955</v>
       </c>
-      <c r="B377" t="s">
+      <c r="B377" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="C377">
+      <c r="C377" s="2">
         <v>2016</v>
       </c>
-      <c r="D377" t="s">
+      <c r="D377" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="E377" t="s">
+      <c r="E377" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="F377" t="s">
+      <c r="F377" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="G377">
+      <c r="G377" s="2">
         <v>751</v>
       </c>
-      <c r="H377">
+      <c r="H377" s="2">
         <v>6</v>
       </c>
-      <c r="I377" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="378" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A378" t="s">
+      <c r="I377" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="378" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A378" s="2" t="s">
         <v>1956</v>
       </c>
-      <c r="B378" t="s">
+      <c r="B378" s="2" t="s">
         <v>1957</v>
       </c>
-      <c r="C378">
+      <c r="C378" s="2">
         <v>2019</v>
       </c>
-      <c r="D378" t="s">
+      <c r="D378" s="2" t="s">
         <v>1958</v>
       </c>
-      <c r="E378" t="s">
+      <c r="E378" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="F378" t="s">
+      <c r="F378" s="2" t="s">
         <v>1959</v>
       </c>
-      <c r="G378">
+      <c r="G378" s="2">
         <v>753</v>
       </c>
-      <c r="H378">
+      <c r="H378" s="2">
         <v>14</v>
       </c>
-      <c r="I378" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="379" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A379" t="s">
+      <c r="I378" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="379" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A379" s="2" t="s">
         <v>1960</v>
       </c>
-      <c r="B379" t="s">
+      <c r="B379" s="2" t="s">
         <v>873</v>
       </c>
-      <c r="C379">
+      <c r="C379" s="2">
         <v>2018</v>
       </c>
-      <c r="D379" t="s">
+      <c r="D379" s="2" t="s">
         <v>874</v>
       </c>
-      <c r="E379" t="s">
+      <c r="E379" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="F379" t="s">
+      <c r="F379" s="2" t="s">
         <v>875</v>
       </c>
-      <c r="G379">
+      <c r="G379" s="2">
         <v>755</v>
       </c>
-      <c r="H379">
+      <c r="H379" s="2">
         <v>26</v>
       </c>
-      <c r="I379" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="380" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A380" t="s">
+      <c r="I379" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="380" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A380" s="2" t="s">
         <v>1961</v>
       </c>
-      <c r="B380" t="s">
+      <c r="B380" s="2" t="s">
         <v>1962</v>
       </c>
-      <c r="C380">
+      <c r="C380" s="2">
         <v>2009</v>
       </c>
-      <c r="D380" t="s">
+      <c r="D380" s="2" t="s">
         <v>1963</v>
       </c>
-      <c r="E380" t="s">
+      <c r="E380" s="2" t="s">
         <v>1964</v>
       </c>
-      <c r="F380" t="s">
+      <c r="F380" s="2" t="s">
         <v>1965</v>
       </c>
-      <c r="G380">
+      <c r="G380" s="2">
         <v>757</v>
       </c>
-      <c r="H380">
+      <c r="H380" s="2">
         <v>109</v>
       </c>
-      <c r="I380" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="381" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A381" t="s">
+      <c r="I380" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="381" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A381" s="2" t="s">
         <v>1966</v>
       </c>
-      <c r="B381" t="s">
+      <c r="B381" s="2" t="s">
         <v>876</v>
       </c>
-      <c r="C381">
+      <c r="C381" s="2">
         <v>2020</v>
       </c>
-      <c r="D381" t="s">
+      <c r="D381" s="2" t="s">
         <v>877</v>
       </c>
-      <c r="E381" t="s">
+      <c r="E381" s="2" t="s">
         <v>878</v>
       </c>
-      <c r="F381" t="s">
+      <c r="F381" s="2" t="s">
         <v>879</v>
       </c>
-      <c r="G381">
+      <c r="G381" s="2">
         <v>759</v>
       </c>
-      <c r="H381">
+      <c r="H381" s="2">
         <v>14</v>
       </c>
-      <c r="I381" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="382" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A382" t="s">
+      <c r="I381" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="382" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A382" s="2" t="s">
         <v>1967</v>
       </c>
-      <c r="B382" t="s">
+      <c r="B382" s="2" t="s">
         <v>1968</v>
       </c>
-      <c r="C382">
+      <c r="C382" s="2">
         <v>2017</v>
       </c>
-      <c r="D382" t="s">
+      <c r="D382" s="2" t="s">
         <v>1969</v>
       </c>
-      <c r="E382" t="s">
+      <c r="E382" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F382" t="s">
+      <c r="F382" s="2" t="s">
         <v>1970</v>
       </c>
-      <c r="G382">
+      <c r="G382" s="2">
         <v>761</v>
       </c>
-      <c r="H382">
+      <c r="H382" s="2">
         <v>137</v>
       </c>
-      <c r="I382" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="383" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A383" t="s">
+      <c r="I382" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="383" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A383" s="2" t="s">
         <v>1971</v>
       </c>
-      <c r="B383" t="s">
+      <c r="B383" s="2" t="s">
         <v>1972</v>
       </c>
-      <c r="C383">
+      <c r="C383" s="2">
         <v>2018</v>
       </c>
-      <c r="D383" t="s">
+      <c r="D383" s="2" t="s">
         <v>1973</v>
       </c>
-      <c r="E383" t="s">
+      <c r="E383" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="F383" t="s">
+      <c r="F383" s="2" t="s">
         <v>1975</v>
       </c>
-      <c r="G383">
+      <c r="G383" s="2">
         <v>763</v>
       </c>
-      <c r="H383">
+      <c r="H383" s="2">
         <v>15</v>
       </c>
-      <c r="I383" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="384" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A384" t="s">
+      <c r="I383" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="384" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A384" s="2" t="s">
         <v>1976</v>
       </c>
-      <c r="B384" t="s">
+      <c r="B384" s="2" t="s">
         <v>1977</v>
       </c>
-      <c r="C384">
+      <c r="C384" s="2">
         <v>2007</v>
       </c>
-      <c r="D384" t="s">
+      <c r="D384" s="2" t="s">
         <v>1978</v>
       </c>
-      <c r="E384" t="s">
+      <c r="E384" s="2" t="s">
         <v>1979</v>
       </c>
-      <c r="F384" t="s">
+      <c r="F384" s="2" t="s">
         <v>1980</v>
       </c>
-      <c r="G384">
+      <c r="G384" s="2">
         <v>765</v>
       </c>
-      <c r="H384">
+      <c r="H384" s="2">
         <v>105</v>
       </c>
-      <c r="I384" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="385" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A385" t="s">
+      <c r="I384" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="385" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A385" s="2" t="s">
         <v>1981</v>
       </c>
-      <c r="B385" t="s">
+      <c r="B385" s="2" t="s">
         <v>880</v>
       </c>
-      <c r="C385">
+      <c r="C385" s="2">
         <v>2013</v>
       </c>
-      <c r="D385" t="s">
+      <c r="D385" s="2" t="s">
         <v>881</v>
       </c>
-      <c r="E385" t="s">
+      <c r="E385" s="2" t="s">
         <v>882</v>
       </c>
-      <c r="F385" t="s">
+      <c r="F385" s="2" t="s">
         <v>883</v>
       </c>
-      <c r="G385">
+      <c r="G385" s="2">
         <v>767</v>
       </c>
-      <c r="H385">
+      <c r="H385" s="2">
         <v>22</v>
       </c>
-      <c r="I385" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="386" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A386" t="s">
+      <c r="I385" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="386" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A386" s="2" t="s">
         <v>1982</v>
       </c>
-      <c r="B386" t="s">
+      <c r="B386" s="2" t="s">
         <v>884</v>
       </c>
-      <c r="C386">
+      <c r="C386" s="2">
         <v>2008</v>
       </c>
-      <c r="D386" t="s">
+      <c r="D386" s="2" t="s">
         <v>885</v>
       </c>
-      <c r="E386" t="s">
+      <c r="E386" s="2" t="s">
         <v>886</v>
       </c>
-      <c r="F386" t="s">
+      <c r="F386" s="2" t="s">
         <v>887</v>
       </c>
-      <c r="G386">
+      <c r="G386" s="2">
         <v>769</v>
       </c>
-      <c r="H386">
+      <c r="H386" s="2">
         <v>7880</v>
       </c>
-      <c r="I386" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="387" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A387" t="s">
+      <c r="I386" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="387" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A387" s="2" t="s">
         <v>1983</v>
       </c>
-      <c r="B387" t="s">
+      <c r="B387" s="2" t="s">
         <v>888</v>
       </c>
-      <c r="C387">
+      <c r="C387" s="2">
         <v>2007</v>
       </c>
-      <c r="D387" t="s">
+      <c r="D387" s="2" t="s">
         <v>889</v>
       </c>
-      <c r="E387" t="s">
+      <c r="E387" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F387" t="s">
+      <c r="F387" s="2" t="s">
         <v>890</v>
       </c>
-      <c r="G387">
+      <c r="G387" s="2">
         <v>771</v>
       </c>
-      <c r="H387">
+      <c r="H387" s="2">
         <v>88</v>
       </c>
-      <c r="I387" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="388" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A388" t="s">
+      <c r="I387" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="388" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A388" s="2" t="s">
         <v>1984</v>
       </c>
-      <c r="B388" t="s">
+      <c r="B388" s="2" t="s">
         <v>1985</v>
       </c>
-      <c r="C388">
+      <c r="C388" s="2">
         <v>2016</v>
       </c>
-      <c r="D388" t="s">
+      <c r="D388" s="2" t="s">
         <v>1986</v>
       </c>
-      <c r="E388" t="s">
+      <c r="E388" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F388" t="s">
+      <c r="F388" s="2" t="s">
         <v>1987</v>
       </c>
-      <c r="G388">
+      <c r="G388" s="2">
         <v>773</v>
       </c>
-      <c r="H388">
+      <c r="H388" s="2">
         <v>74</v>
       </c>
-      <c r="I388" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="389" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A389" t="s">
+      <c r="I388" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="389" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A389" s="2" t="s">
         <v>1988</v>
       </c>
-      <c r="B389" t="s">
+      <c r="B389" s="2" t="s">
         <v>1989</v>
       </c>
-      <c r="C389">
+      <c r="C389" s="2">
         <v>2011</v>
       </c>
-      <c r="D389" t="s">
+      <c r="D389" s="2" t="s">
         <v>1990</v>
       </c>
-      <c r="E389" t="s">
+      <c r="E389" s="2" t="s">
         <v>1991</v>
       </c>
-      <c r="F389" t="s">
+      <c r="F389" s="2" t="s">
         <v>1992</v>
       </c>
-      <c r="G389">
+      <c r="G389" s="2">
         <v>775</v>
       </c>
-      <c r="H389">
+      <c r="H389" s="2">
         <v>78</v>
       </c>
-      <c r="I389" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="390" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A390" t="s">
+      <c r="I389" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="390" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A390" s="2" t="s">
         <v>1993</v>
       </c>
-      <c r="B390" t="s">
+      <c r="B390" s="2" t="s">
         <v>1994</v>
       </c>
-      <c r="C390">
+      <c r="C390" s="2">
         <v>2009</v>
       </c>
-      <c r="D390" t="s">
+      <c r="D390" s="2" t="s">
         <v>1995</v>
       </c>
-      <c r="E390" t="s">
+      <c r="E390" s="2" t="s">
         <v>1996</v>
       </c>
-      <c r="F390" t="s">
+      <c r="F390" s="2" t="s">
         <v>1997</v>
       </c>
-      <c r="G390">
+      <c r="G390" s="2">
         <v>777</v>
       </c>
-      <c r="H390">
+      <c r="H390" s="2">
         <v>97</v>
       </c>
-      <c r="I390" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="391" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A391" t="s">
+      <c r="I390" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="391" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A391" s="2" t="s">
         <v>1998</v>
       </c>
-      <c r="B391" t="s">
+      <c r="B391" s="2" t="s">
         <v>1999</v>
       </c>
-      <c r="C391">
+      <c r="C391" s="2">
         <v>2017</v>
       </c>
-      <c r="D391" t="s">
+      <c r="D391" s="2" t="s">
         <v>2000</v>
       </c>
-      <c r="E391" t="s">
+      <c r="E391" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="F391" t="s">
+      <c r="F391" s="2" t="s">
         <v>2001</v>
       </c>
-      <c r="G391">
+      <c r="G391" s="2">
         <v>779</v>
       </c>
-      <c r="H391">
+      <c r="H391" s="2">
         <v>18</v>
       </c>
-      <c r="I391" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="392" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A392" t="s">
+      <c r="I391" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="392" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A392" s="2" t="s">
         <v>2002</v>
       </c>
-      <c r="B392" t="s">
+      <c r="B392" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="C392">
+      <c r="C392" s="2">
         <v>2018</v>
       </c>
-      <c r="D392" t="s">
+      <c r="D392" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="E392" t="s">
+      <c r="E392" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="F392" t="s">
+      <c r="F392" s="2" t="s">
         <v>892</v>
       </c>
-      <c r="G392">
+      <c r="G392" s="2">
         <v>781</v>
       </c>
-      <c r="H392">
+      <c r="H392" s="2">
         <v>11</v>
       </c>
-      <c r="I392" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="393" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A393" t="s">
+      <c r="I392" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="393" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A393" s="2" t="s">
         <v>2003</v>
       </c>
-      <c r="B393" t="s">
+      <c r="B393" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="C393">
+      <c r="C393" s="2">
         <v>2017</v>
       </c>
-      <c r="D393" t="s">
+      <c r="D393" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="E393" t="s">
+      <c r="E393" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="F393" t="s">
+      <c r="F393" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="G393">
+      <c r="G393" s="2">
         <v>783</v>
       </c>
-      <c r="H393">
+      <c r="H393" s="2">
         <v>14</v>
       </c>
-      <c r="I393" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="394" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A394" t="s">
+      <c r="I393" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="394" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A394" s="2" t="s">
         <v>2004</v>
       </c>
-      <c r="B394" t="s">
+      <c r="B394" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="C394">
+      <c r="C394" s="2">
         <v>2011</v>
       </c>
-      <c r="D394" t="s">
+      <c r="D394" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="E394" t="s">
+      <c r="E394" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="F394" t="s">
+      <c r="F394" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="G394">
+      <c r="G394" s="2">
         <v>785</v>
       </c>
-      <c r="H394">
+      <c r="H394" s="2">
         <v>69</v>
       </c>
-      <c r="I394" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="395" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A395" t="s">
+      <c r="I394" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="395" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A395" s="2" t="s">
         <v>2005</v>
       </c>
-      <c r="B395" t="s">
+      <c r="B395" s="2" t="s">
         <v>2006</v>
       </c>
-      <c r="C395">
+      <c r="C395" s="2">
         <v>2019</v>
       </c>
-      <c r="D395" t="s">
+      <c r="D395" s="2" t="s">
         <v>2007</v>
       </c>
-      <c r="E395" t="s">
+      <c r="E395" s="2" t="s">
         <v>2008</v>
       </c>
-      <c r="F395" t="s">
+      <c r="F395" s="2" t="s">
         <v>2009</v>
       </c>
-      <c r="G395">
+      <c r="G395" s="2">
         <v>787</v>
       </c>
-      <c r="H395">
+      <c r="H395" s="2">
         <v>4</v>
       </c>
-      <c r="I395" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="396" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A396" t="s">
+      <c r="I395" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="396" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A396" s="2" t="s">
         <v>2010</v>
       </c>
-      <c r="B396" t="s">
+      <c r="B396" s="2" t="s">
         <v>2011</v>
       </c>
-      <c r="C396">
+      <c r="C396" s="2">
         <v>2010</v>
       </c>
-      <c r="D396" t="s">
+      <c r="D396" s="2" t="s">
         <v>2012</v>
       </c>
-      <c r="E396" t="s">
+      <c r="E396" s="2" t="s">
         <v>2013</v>
       </c>
-      <c r="F396" t="s">
+      <c r="F396" s="2" t="s">
         <v>2014</v>
       </c>
-      <c r="G396">
+      <c r="G396" s="2">
         <v>789</v>
       </c>
-      <c r="H396">
+      <c r="H396" s="2">
         <v>101</v>
       </c>
-      <c r="I396" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="397" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A397" t="s">
+      <c r="I396" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="397" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A397" s="2" t="s">
         <v>2015</v>
       </c>
-      <c r="B397" t="s">
+      <c r="B397" s="2" t="s">
         <v>2016</v>
       </c>
-      <c r="C397">
+      <c r="C397" s="2">
         <v>2014</v>
       </c>
-      <c r="D397" t="s">
+      <c r="D397" s="2" t="s">
         <v>2017</v>
       </c>
-      <c r="E397" t="s">
+      <c r="E397" s="2" t="s">
         <v>652</v>
       </c>
-      <c r="F397" t="s">
+      <c r="F397" s="2" t="s">
         <v>2018</v>
       </c>
-      <c r="G397">
+      <c r="G397" s="2">
         <v>791</v>
       </c>
-      <c r="H397">
+      <c r="H397" s="2">
         <v>4</v>
       </c>
-      <c r="I397" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="398" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A398" t="s">
+      <c r="I397" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="398" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A398" s="2" t="s">
         <v>2019</v>
       </c>
-      <c r="B398" t="s">
+      <c r="B398" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="C398">
+      <c r="C398" s="2">
         <v>2018</v>
       </c>
-      <c r="D398" t="s">
+      <c r="D398" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="E398" t="s">
+      <c r="E398" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F398" t="s">
+      <c r="F398" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="G398">
+      <c r="G398" s="2">
         <v>793</v>
       </c>
-      <c r="H398">
+      <c r="H398" s="2">
         <v>74</v>
       </c>
-      <c r="I398" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="399" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A399" t="s">
+      <c r="I398" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="399" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A399" s="2" t="s">
         <v>2020</v>
       </c>
-      <c r="B399" t="s">
+      <c r="B399" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="C399">
+      <c r="C399" s="2">
         <v>2010</v>
       </c>
-      <c r="D399" t="s">
+      <c r="D399" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="E399" t="s">
+      <c r="E399" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="F399" t="s">
+      <c r="F399" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="G399">
+      <c r="G399" s="2">
         <v>795</v>
       </c>
-      <c r="H399">
+      <c r="H399" s="2">
         <v>238</v>
       </c>
-      <c r="I399" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="400" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A400" t="s">
+      <c r="I399" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="400" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A400" s="2" t="s">
         <v>2021</v>
       </c>
-      <c r="B400" t="s">
+      <c r="B400" s="2" t="s">
         <v>893</v>
       </c>
-      <c r="C400">
+      <c r="C400" s="2">
         <v>2017</v>
       </c>
-      <c r="D400" t="s">
+      <c r="D400" s="2" t="s">
         <v>894</v>
       </c>
-      <c r="E400" t="s">
+      <c r="E400" s="2" t="s">
         <v>895</v>
       </c>
-      <c r="F400" t="s">
+      <c r="F400" s="2" t="s">
         <v>896</v>
       </c>
-      <c r="G400">
+      <c r="G400" s="2">
         <v>797</v>
       </c>
-      <c r="H400">
-        <v>13</v>
-      </c>
-      <c r="I400" t="s">
+      <c r="H400" s="2">
+        <v>13</v>
+      </c>
+      <c r="I400" s="2" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>